<commit_message>
[SCH][PCB] Combine delay PCB with integrated PCB; Include 2 pressure sensors and 1 gyro; Remove redundant 4 pin molex; Add 2 pin molex for regulated 5V output; Add 100R pulldown resistor
</commit_message>
<xml_diff>
--- a/Altium/2017_Avionics_Integrated_PCB/Project Outputs for 2017_Avionics_Integrated_PCB/2017_Avionics_Integrated_PCB.xlsx
+++ b/Altium/2017_Avionics_Integrated_PCB/Project Outputs for 2017_Avionics_Integrated_PCB/2017_Avionics_Integrated_PCB.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="66">
   <si>
     <t>Description</t>
   </si>
@@ -45,10 +45,10 @@
     <t>Supplier Subtotal 1</t>
   </si>
   <si>
-    <t>Teensy 3.2 Development Board, The SparkFun MPU-9250 IMU Breakout features the latest 9-axis MEMS sensor from InvenSense., The MPL3115A2 is a MEMS pressure sensor that provides Altitude data to within 30cm (with oversampling enabled)., The SparkFun MPU-9250 IMU Breakout features the latest 9-axis MEMS sensor from InvenSense., The MPL3115A2 is a MEMS pressure sensor that provides Altitude data to within 30cm (with oversampling enabled).</t>
-  </si>
-  <si>
-    <t>U2, U4, U5, U7, U8</t>
+    <t>Teensy 3.2 Development Board, The SparkFun MPU-9250 IMU Breakout features the latest 9-axis MEMS sensor from InvenSense., The MPL3115A2 is a MEMS pressure sensor that provides Altitude data to within 30cm (with oversampling enabled)., The MPL3115A2 is a MEMS pressure sensor that provides Altitude data to within 30cm (with oversampling enabled).</t>
+  </si>
+  <si>
+    <t>U2, U4, U5, U7</t>
   </si>
   <si>
     <t/>
@@ -69,10 +69,10 @@
     <t>Digi-Key</t>
   </si>
   <si>
-    <t>Teensy Battery, [NoValue], [NoValue]</t>
-  </si>
-  <si>
-    <t>P1, P2, P4</t>
+    <t>Teensy Battery, [NoValue], [NoValue], [NoValue]</t>
+  </si>
+  <si>
+    <t>P1, P2, P4, P7</t>
   </si>
   <si>
     <t>Molex, LLC</t>
@@ -84,7 +84,7 @@
     <t>Header, 4-Pin</t>
   </si>
   <si>
-    <t>P5, P6, P7</t>
+    <t>P5, P6</t>
   </si>
   <si>
     <t>P3</t>
@@ -118,6 +118,12 @@
   </si>
   <si>
     <t>ERJ-3EKF8873V</t>
+  </si>
+  <si>
+    <t>R3</t>
+  </si>
+  <si>
+    <t>ERJ-PA3F1000V</t>
   </si>
   <si>
     <t>Panasonic ERJ-PA3F1001V, Panasonic ERJ-PA3F1001V, Panasonic ERJ-PA3F1001V, Vishay CRCW060347R0FKEAHP</t>
@@ -571,7 +577,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H19"/>
+  <dimension ref="A1:H20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -619,7 +625,7 @@
         <v>9</v>
       </c>
       <c r="C2" s="3">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D2" s="4"/>
       <c r="E2" s="4"/>
@@ -663,7 +669,7 @@
         <v>17</v>
       </c>
       <c r="C4" s="3">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D4" s="4" t="s">
         <v>18</v>
@@ -678,7 +684,7 @@
         <v>1.26</v>
       </c>
       <c r="H4" s="3">
-        <v>3.78</v>
+        <v>5.04</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
@@ -689,7 +695,7 @@
         <v>21</v>
       </c>
       <c r="C5" s="3">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D5" s="4" t="s">
         <v>18</v>
@@ -704,7 +710,7 @@
         <v>1.88</v>
       </c>
       <c r="H5" s="3">
-        <v>5.64</v>
+        <v>3.76</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.3">
@@ -813,19 +819,19 @@
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B10" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="B10" s="2" t="s">
-        <v>34</v>
-      </c>
       <c r="C10" s="3">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D10" s="4" t="s">
         <v>31</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F10" s="2" t="s">
         <v>15</v>
@@ -834,24 +840,24 @@
         <v>0.23</v>
       </c>
       <c r="H10" s="3">
-        <v>0.92</v>
+        <v>0.23</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B11" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="B11" s="2" t="s">
-        <v>37</v>
-      </c>
       <c r="C11" s="3">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D11" s="4" t="s">
         <v>31</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F11" s="2" t="s">
         <v>15</v>
@@ -860,18 +866,18 @@
         <v>0.23</v>
       </c>
       <c r="H11" s="3">
-        <v>0.69</v>
+        <v>0.92</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
-        <v>29</v>
+        <v>38</v>
       </c>
       <c r="B12" s="2" t="s">
         <v>39</v>
       </c>
       <c r="C12" s="3">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D12" s="4" t="s">
         <v>31</v>
@@ -886,7 +892,7 @@
         <v>0.23</v>
       </c>
       <c r="H12" s="3">
-        <v>0.23</v>
+        <v>0.69</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.3">
@@ -897,7 +903,7 @@
         <v>41</v>
       </c>
       <c r="C13" s="3">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D13" s="4" t="s">
         <v>31</v>
@@ -912,7 +918,7 @@
         <v>0.23</v>
       </c>
       <c r="H13" s="3">
-        <v>0.69</v>
+        <v>0.23</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.3">
@@ -923,7 +929,7 @@
         <v>43</v>
       </c>
       <c r="C14" s="3">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D14" s="4" t="s">
         <v>31</v>
@@ -938,136 +944,162 @@
         <v>0.23</v>
       </c>
       <c r="H14" s="3">
-        <v>0.23</v>
+        <v>0.69</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B15" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="B15" s="2" t="s">
+      <c r="C15" s="3">
+        <v>1</v>
+      </c>
+      <c r="D15" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="E15" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="C15" s="3">
-        <v>4</v>
-      </c>
-      <c r="D15" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="E15" s="4" t="s">
-        <v>48</v>
-      </c>
       <c r="F15" s="2" t="s">
         <v>15</v>
       </c>
       <c r="G15" s="3">
-        <v>1.37</v>
+        <v>0.23</v>
       </c>
       <c r="H15" s="3">
-        <v>5.48</v>
+        <v>0.23</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="C16" s="3">
+        <v>4</v>
+      </c>
+      <c r="D16" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="B16" s="2" t="s">
+      <c r="E16" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="C16" s="3">
-        <v>1</v>
-      </c>
-      <c r="D16" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="E16" s="4" t="s">
-        <v>52</v>
-      </c>
       <c r="F16" s="2" t="s">
         <v>15</v>
       </c>
       <c r="G16" s="3">
-        <v>0.97</v>
+        <v>1.37</v>
       </c>
       <c r="H16" s="3">
-        <v>0.97</v>
+        <v>5.48</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="C17" s="3">
+        <v>1</v>
+      </c>
+      <c r="D17" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="B17" s="2" t="s">
+      <c r="E17" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="C17" s="3">
-        <v>2</v>
-      </c>
-      <c r="D17" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="E17" s="4" t="s">
-        <v>55</v>
-      </c>
       <c r="F17" s="2" t="s">
         <v>15</v>
       </c>
       <c r="G17" s="3">
-        <v>1.1299999999999999</v>
+        <v>0.97</v>
       </c>
       <c r="H17" s="3">
-        <v>2.2599999999999998</v>
+        <v>0.97</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="B18" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="B18" s="2" t="s">
+      <c r="C18" s="3">
+        <v>2</v>
+      </c>
+      <c r="D18" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="E18" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="C18" s="3">
-        <v>1</v>
-      </c>
-      <c r="D18" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="E18" s="4" t="s">
-        <v>59</v>
-      </c>
       <c r="F18" s="2" t="s">
         <v>15</v>
       </c>
       <c r="G18" s="3">
-        <v>5.24</v>
+        <v>1.1299999999999999</v>
       </c>
       <c r="H18" s="3">
-        <v>5.24</v>
+        <v>2.2599999999999998</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C19" s="3">
         <v>1</v>
       </c>
       <c r="D19" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="E19" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="F19" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="G19" s="3">
+        <v>5.24</v>
+      </c>
+      <c r="H19" s="3">
+        <v>5.24</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A20" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="E19" s="4" t="s">
+      <c r="B20" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="F19" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="G19" s="3">
+      <c r="C20" s="3">
+        <v>1</v>
+      </c>
+      <c r="D20" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="E20" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="F20" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="G20" s="3">
         <v>0.66</v>
       </c>
-      <c r="H19" s="3">
+      <c r="H20" s="3">
         <v>0.66</v>
       </c>
     </row>
@@ -1109,8 +1141,10 @@
     <hyperlink ref="E18" r:id="rId32" tooltip="Manufacturer"/>
     <hyperlink ref="D19" r:id="rId33" tooltip="Component"/>
     <hyperlink ref="E19" r:id="rId34" tooltip="Manufacturer"/>
+    <hyperlink ref="D20" r:id="rId35" tooltip="Component"/>
+    <hyperlink ref="E20" r:id="rId36" tooltip="Manufacturer"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId35"/>
+  <pageSetup orientation="portrait" r:id="rId37"/>
 </worksheet>
 </file>
</xml_diff>